<commit_message>
modified dashboard for release on Shiny.io
</commit_message>
<xml_diff>
--- a/data/Negociado_de_Policia/INCIDENTES DE VIOLENCIA DOMÉSTICA POR ÁREA.xlsx
+++ b/data/Negociado_de_Policia/INCIDENTES DE VIOLENCIA DOMÉSTICA POR ÁREA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frankie.rodriguez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixbaez822/Desktop/ViolenciaGeneroPR/data/Negociado_de_Policia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFC0E31-2B31-4B2B-9689-C8D4CBAE5196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4A417F-A4B5-F646-8A6B-AE1B94D157AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DF55321F-32D2-4711-8A63-1FF4D970C60B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20740" windowHeight="14320" xr2:uid="{DF55321F-32D2-4711-8A63-1FF4D970C60B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,9 +264,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -304,7 +304,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -410,7 +410,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -552,7 +552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -563,19 +563,19 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="24.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="24.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
@@ -584,7 +584,7 @@
       <c r="G1" s="9"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D2" s="11" t="s">
         <v>17</v>
       </c>
@@ -593,7 +593,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -601,7 +601,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -611,7 +611,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -621,7 +621,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -631,7 +631,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
@@ -641,7 +641,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
@@ -651,7 +651,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -661,7 +661,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -671,7 +671,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -681,7 +681,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
@@ -691,7 +691,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -701,7 +701,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -711,7 +711,7 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -721,7 +721,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -731,7 +731,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="6">
         <v>6080</v>

</xml_diff>